<commit_message>
Updated dynamic component render
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lohith_R\Documents\LatestCode\react-magneto-v1-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lohith_R\Documents\LatestCode\react-magneto-v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6551189-8156-435C-B0C4-E36853E90811}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2334D8-A1D0-46B9-A335-E3965611A184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +658,9 @@
       <c r="G5" t="s">
         <v>38</v>
       </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
       <c r="K5" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Using Flex box for componet layout
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\react-projects\react-magneto-v1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
   <si>
     <t>Components</t>
   </si>
@@ -83,9 +78,6 @@
     <t>className</t>
   </si>
   <si>
-    <t>textcontainerTrv</t>
-  </si>
-  <si>
     <t>TextInput</t>
   </si>
   <si>
@@ -95,9 +87,6 @@
     <t xml:space="preserve">Customer First Name: </t>
   </si>
   <si>
-    <t>textCompTrv</t>
-  </si>
-  <si>
     <t>custLastName</t>
   </si>
   <si>
@@ -215,36 +204,6 @@
     <t>Pie</t>
   </si>
   <si>
-    <t>DatePicker</t>
-  </si>
-  <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>MM/dd/yyyy</t>
-  </si>
-  <si>
-    <t>Date of Birth:</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>SearchField</t>
-  </si>
-  <si>
-    <t>sicCode</t>
-  </si>
-  <si>
-    <t>SIC Code</t>
-  </si>
-  <si>
-    <t>SIC Code:</t>
-  </si>
-  <si>
-    <t>placeHolder</t>
-  </si>
-  <si>
     <t>api</t>
   </si>
   <si>
@@ -254,20 +213,26 @@
     <t>library</t>
   </si>
   <si>
+    <t>DemoApp</t>
+  </si>
+  <si>
+    <t>Customer Information</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>child-row</t>
+  </si>
+  <si>
     <t>primeReact</t>
-  </si>
-  <si>
-    <t>DemoApp</t>
-  </si>
-  <si>
-    <t>Customer Information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,35 +536,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="75.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="75.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -649,21 +614,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -671,411 +636,376 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O4" t="s">
         <v>18</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O6" t="s">
         <v>18</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="O8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="P9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
       <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
         <v>34</v>
-      </c>
-      <c r="G10" t="s">
-        <v>36</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="K10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
         <v>51</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G12" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
         <v>53</v>
       </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
         <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
         <v>53</v>
       </c>
-      <c r="G13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>70</v>
-      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>